<commit_message>
fixed data to excel issue
tried making the create excel a function, but it works better if its in the main
</commit_message>
<xml_diff>
--- a/test_data.pkl_converted_data.xlsx
+++ b/test_data.pkl_converted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +448,326 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>design</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Test Prop 1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2016-12-05</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2016-12-08</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>design</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Test Prop 2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2016-12-13</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2016-12-16</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test Prop 1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2016-12-19</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2017-01-23</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Test Prop 2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2016-12-23</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2017-01-23</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>design</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Test Prop 2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2017-01-09</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2017-01-12</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Test Prop 3</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2017-01-23</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2017-02-10</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Test Prop 4</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2017-01-23</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2017-02-07</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Test Prop 5</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2017-01-26</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2017-02-08</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>duplicate build</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Test Prop 1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2017-03-20</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2017-03-24</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>duplicate build</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Test Prop 2</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Horace's Home 2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2017-03-20</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2017-03-24</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>teehee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Possibly done revising challenge 1
Will have to take a look tomorrow to be sure
</commit_message>
<xml_diff>
--- a/test_data.pkl_converted_data.xlsx
+++ b/test_data.pkl_converted_data.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,13 +25,39 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <color rgb="00ffffff"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <color rgb="008B0000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <i val="1"/>
+      <color rgb="008B0000"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +72,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,358 +451,315 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="19" customWidth="1" min="1" max="1"/>
+    <col width="19.5" customWidth="1" min="2" max="2"/>
+    <col width="21.5" customWidth="1" min="3" max="3"/>
+    <col width="20.5" customWidth="1" min="4" max="4"/>
+    <col width="19.5" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Task</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Set Part</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Parent Build</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Start Date</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>End Date</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>design</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Test Prop 1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Horace's Home</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>2016-12-05</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>2016-12-08</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>teehee</t>
-        </is>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>design</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Test Prop 2</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Horace's Home</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>2016-12-13</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>2016-12-16</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>teehee</t>
-        </is>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>first build</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Test Prop 1</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>Horace's Home</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>2016-12-19</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>2017-01-23</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>teehee</t>
-        </is>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>first build</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Test Prop 2</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>Horace's Home</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>2016-12-23</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>2017-01-23</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>teehee</t>
-        </is>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>design</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>Test Prop 2</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>Horace's Home</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>2017-01-09</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
         <is>
           <t>2017-01-12</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>teehee</t>
-        </is>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>first build</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Test Prop 3</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>Horace's Home</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>2017-01-23</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>2017-02-10</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>teehee</t>
-        </is>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>first build</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>Test Prop 4</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="4" t="inlineStr">
         <is>
           <t>Not available</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>2017-01-23</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr">
         <is>
           <t>2017-02-07</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>teehee</t>
-        </is>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>first build</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>Test Prop 5</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>Horace's Home</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>2017-01-26</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="3" t="inlineStr">
         <is>
           <t>2017-02-08</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>teehee</t>
-        </is>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>duplicate build</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>Test Prop 1</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>Horace's Home</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>2017-03-20</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="3" t="inlineStr">
         <is>
           <t>2017-03-24</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>teehee</t>
-        </is>
-      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>duplicate build</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>Test Prop 2</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>Horace's Home 2</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>2017-03-20</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>2017-03-24</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>teehee</t>
         </is>
       </c>
     </row>

</xml_diff>